<commit_message>
Added "summer day" song
</commit_message>
<xml_diff>
--- a/app/src/main/assets/samples/sources.xlsx
+++ b/app/src/main/assets/samples/sources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android Studio Projects\Projects\Calmify\app\src\main\assets\music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android Studio Projects\Projects\Calmify\app\src\main\assets\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Song</t>
   </si>
@@ -75,13 +75,25 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by-sa/3.0/us/</t>
+  </si>
+  <si>
+    <t>Summer Day</t>
+  </si>
+  <si>
+    <t>Summer Day Kevin MacLeod (incompetech.com)</t>
+  </si>
+  <si>
+    <t>Licensed under Creative Commons: By Attribution 3.0 License</t>
+  </si>
+  <si>
+    <t>http://creativecommons.org/licenses/by/3.0/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +108,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,6 +179,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +473,7 @@
     <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -467,7 +487,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -475,7 +495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -483,7 +503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -493,8 +513,11 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -507,8 +530,11 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -520,6 +546,20 @@
       </c>
       <c r="D6" t="s">
         <v>15</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>